<commit_message>
refactor; update Alice sheet
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC4798-4D7E-41A5-AFCD-B1E1EECB5BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC40A7C-7C21-4F34-8AC5-85E8090600A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="128">
   <si>
     <t>role</t>
   </si>
@@ -9968,8 +9968,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23839,8 +23839,8 @@
   </sheetPr>
   <dimension ref="A1:X1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="A12:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23905,7 +23905,6 @@
       <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -23928,64 +23927,44 @@
     </row>
     <row r="6" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" t="s">
         <v>79</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D9" t="s">
         <v>77</v>
       </c>
     </row>
+    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
tests: fix bugs and get tests to pass
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A8C20C-BE05-4B53-82A0-A0B23A0BFB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373D6C46-DE23-4B48-B558-D135A94F5D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="137">
   <si>
     <t>role</t>
   </si>
@@ -213,13 +213,7 @@
     <t>TransmissionSubstation</t>
   </si>
   <si>
-    <t>power:TransmissionSubstation</t>
-  </si>
-  <si>
     <t>DistributionSubstation</t>
-  </si>
-  <si>
-    <t>power:DistributionSubstation</t>
   </si>
   <si>
     <t>PowerLine</t>
@@ -241,9 +235,6 @@
   </si>
   <si>
     <t>Transmission</t>
-  </si>
-  <si>
-    <t>power:Transmission</t>
   </si>
   <si>
     <t>EnergyConsumer</t>
@@ -369,9 +360,6 @@
     <t>power:EnergyArea(version=0.1.0)</t>
   </si>
   <si>
-    <t>windTurbine</t>
-  </si>
-  <si>
     <t>power:WindFarm(version=0.1.0)</t>
   </si>
   <si>
@@ -416,6 +404,42 @@
   <si>
     <t>windTurbines</t>
   </si>
+  <si>
+    <t>power:TransmissionSubstation(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:DistributionSubstation(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:ArrayCable(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:ExportCable(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:Transmission(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:EnergyConsumer(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:GeoLocation(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:CircuitBreaker(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:CurrentTransformer(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:DisconnectSwitch(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:VoltageLevel(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:VoltageTransformer(version=0.1.0)</t>
+  </si>
 </sst>
 </file>
 
@@ -424,11 +448,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -561,54 +592,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8698,28 +8730,28 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="7.44140625" customWidth="1"/>
     <col min="7" max="24" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -8763,7 +8795,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -8772,10 +8804,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>52</v>
+        <v>94</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -8783,7 +8815,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -8792,10 +8824,10 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8803,7 +8835,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -8812,10 +8844,10 @@
         <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8823,123 +8855,123 @@
         <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8947,39 +8979,39 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9973,8 +10005,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10003,23 +10035,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
@@ -10099,13 +10131,13 @@
         <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
@@ -10119,7 +10151,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -10134,16 +10166,16 @@
         <v>52</v>
       </c>
       <c r="K4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="N4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
@@ -10174,7 +10206,7 @@
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M5" t="s">
         <v>30</v>
@@ -10189,10 +10221,10 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
@@ -10204,19 +10236,19 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J6" t="s">
         <v>52</v>
       </c>
       <c r="K6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
@@ -10252,7 +10284,7 @@
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="M8" t="s">
         <v>26</v>
@@ -10285,7 +10317,7 @@
         <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="M9" t="s">
         <v>27</v>
@@ -10314,7 +10346,7 @@
         <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="M10" t="s">
         <v>31</v>
@@ -10329,10 +10361,10 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
         <v>37</v>
@@ -10347,13 +10379,13 @@
         <v>53</v>
       </c>
       <c r="K11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="M11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
@@ -10365,10 +10397,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -10380,25 +10412,25 @@
         <v>53</v>
       </c>
       <c r="K12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="M12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
         <v>37</v>
@@ -10410,13 +10442,13 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K14" t="s">
         <v>38</v>
       </c>
       <c r="L14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M14" t="s">
         <v>38</v>
@@ -10428,13 +10460,13 @@
     </row>
     <row r="15" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
         <v>37</v>
@@ -10446,16 +10478,16 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
@@ -10464,10 +10496,10 @@
     </row>
     <row r="16" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -10479,16 +10511,16 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -10524,7 +10556,7 @@
         <v>23</v>
       </c>
       <c r="L18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M18" t="s">
         <v>23</v>
@@ -10557,7 +10589,7 @@
         <v>25</v>
       </c>
       <c r="L19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M19" t="s">
         <v>25</v>
@@ -10568,10 +10600,10 @@
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
         <v>35</v>
@@ -10583,10 +10615,10 @@
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
@@ -10601,7 +10633,7 @@
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
         <v>35</v>
@@ -10613,7 +10645,7 @@
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M21" t="s">
         <v>43</v>
@@ -10628,10 +10660,10 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
         <v>35</v>
@@ -10643,10 +10675,10 @@
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
@@ -10656,10 +10688,10 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
         <v>37</v>
@@ -10674,13 +10706,13 @@
         <v>57</v>
       </c>
       <c r="K23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L23" t="s">
+        <v>100</v>
+      </c>
+      <c r="M23" t="s">
         <v>103</v>
-      </c>
-      <c r="M23" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10688,10 +10720,10 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
         <v>37</v>
@@ -10706,13 +10738,13 @@
         <v>57</v>
       </c>
       <c r="K24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
@@ -10724,10 +10756,10 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
         <v>37</v>
@@ -10742,13 +10774,13 @@
         <v>57</v>
       </c>
       <c r="K25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
@@ -10760,7 +10792,7 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -10775,13 +10807,13 @@
         <v>57</v>
       </c>
       <c r="K26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10789,7 +10821,7 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -10804,13 +10836,13 @@
         <v>57</v>
       </c>
       <c r="K27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
@@ -10828,10 +10860,10 @@
         <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>35</v>
@@ -10843,10 +10875,10 @@
         <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
@@ -10858,10 +10890,10 @@
         <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
         <v>37</v>
@@ -10876,13 +10908,13 @@
         <v>59</v>
       </c>
       <c r="K30" t="s">
+        <v>105</v>
+      </c>
+      <c r="L30" t="s">
         <v>108</v>
       </c>
-      <c r="L30" t="s">
-        <v>111</v>
-      </c>
       <c r="M30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
@@ -10918,7 +10950,7 @@
         <v>23</v>
       </c>
       <c r="L32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M32" t="s">
         <v>23</v>
@@ -10933,10 +10965,10 @@
         <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
         <v>37</v>
@@ -10951,13 +10983,13 @@
         <v>55</v>
       </c>
       <c r="K33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L33" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R33" s="11"/>
       <c r="S33" s="11"/>
@@ -10987,7 +11019,7 @@
         <v>27</v>
       </c>
       <c r="L34" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M34" t="s">
         <v>27</v>
@@ -11016,7 +11048,7 @@
         <v>30</v>
       </c>
       <c r="L35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M35" t="s">
         <v>30</v>
@@ -11037,7 +11069,7 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D37" t="s">
         <v>53</v>
@@ -11052,10 +11084,10 @@
         <v>1</v>
       </c>
       <c r="L37" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M37" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="R37" s="10"/>
       <c r="S37" s="11"/>
@@ -11067,7 +11099,7 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D38" t="s">
         <v>59</v>
@@ -11085,13 +11117,13 @@
         <v>56</v>
       </c>
       <c r="K38" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L38" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M38" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="R38" s="10"/>
       <c r="S38" s="11"/>
@@ -11103,10 +11135,10 @@
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
         <v>35</v>
@@ -11118,10 +11150,10 @@
         <v>1</v>
       </c>
       <c r="L39" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M39" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="R39" s="10"/>
     </row>
@@ -11130,10 +11162,10 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
         <v>37</v>
@@ -11148,19 +11180,19 @@
         <v>56</v>
       </c>
       <c r="K40" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M40" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
@@ -11175,13 +11207,13 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K42" t="s">
         <v>23</v>
       </c>
       <c r="L42" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M42" t="s">
         <v>23</v>
@@ -11189,13 +11221,13 @@
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E43" t="s">
         <v>37</v>
@@ -11207,13 +11239,13 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K43" t="s">
         <v>25</v>
       </c>
       <c r="L43" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M43" t="s">
         <v>25</v>
@@ -11221,10 +11253,10 @@
     </row>
     <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -11236,25 +11268,25 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K44" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L44" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M44" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D46" t="s">
         <v>28</v>
@@ -11266,24 +11298,24 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="L46" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="M46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D47" t="s">
         <v>28</v>
@@ -11295,28 +11327,28 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K47" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L47" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="M47" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E49" t="s">
         <v>35</v>
@@ -11328,22 +11360,22 @@
         <v>1</v>
       </c>
       <c r="L49" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M49" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E51" t="s">
         <v>35</v>
@@ -11355,10 +11387,10 @@
         <v>1</v>
       </c>
       <c r="L51" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="M51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -23842,15 +23874,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X1002"/>
+  <dimension ref="A1:X1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="A3:D9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
@@ -23859,12 +23892,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -23924,56 +23957,73 @@
     </row>
     <row r="5" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
         <v>74</v>
       </c>
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -24951,6 +25001,8 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
refactor: fix small bug
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373D6C46-DE23-4B48-B558-D135A94F5D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E11DB8C-5CB4-45E7-B56C-6B8BE8DD01D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10005,8 +10005,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10608,12 +10608,6 @@
       <c r="E20" t="s">
         <v>35</v>
       </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
       <c r="L20" t="s">
         <v>100</v>
       </c>
@@ -10638,12 +10632,6 @@
       <c r="E21" t="s">
         <v>35</v>
       </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
       <c r="L21" t="s">
         <v>100</v>
       </c>
@@ -10667,12 +10655,6 @@
       </c>
       <c r="E22" t="s">
         <v>35</v>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" t="b">
-        <v>1</v>
       </c>
       <c r="L22" t="s">
         <v>100</v>
@@ -10868,12 +10850,6 @@
       <c r="E29" t="s">
         <v>35</v>
       </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-      <c r="G29" t="b">
-        <v>1</v>
-      </c>
       <c r="L29" t="s">
         <v>108</v>
       </c>
@@ -11077,12 +11053,6 @@
       <c r="E37" t="s">
         <v>35</v>
       </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
       <c r="L37" t="s">
         <v>110</v>
       </c>
@@ -11143,12 +11113,6 @@
       <c r="E39" t="s">
         <v>35</v>
       </c>
-      <c r="F39" t="b">
-        <v>0</v>
-      </c>
-      <c r="G39" t="b">
-        <v>1</v>
-      </c>
       <c r="L39" t="s">
         <v>110</v>
       </c>
@@ -11353,12 +11317,6 @@
       <c r="E49" t="s">
         <v>35</v>
       </c>
-      <c r="F49" t="b">
-        <v>0</v>
-      </c>
-      <c r="G49" t="b">
-        <v>1</v>
-      </c>
       <c r="L49" t="s">
         <v>120</v>
       </c>
@@ -11379,12 +11337,6 @@
       </c>
       <c r="E51" t="s">
         <v>35</v>
-      </c>
-      <c r="F51" t="b">
-        <v>0</v>
-      </c>
-      <c r="G51" t="b">
-        <v>1</v>
       </c>
       <c r="L51" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
fix: Alice direct nullable
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E11DB8C-5CB4-45E7-B56C-6B8BE8DD01D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59381834-3652-49EC-87E8-A7FF298D3CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10005,8 +10005,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10230,7 +10230,7 @@
         <v>37</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -10370,7 +10370,7 @@
         <v>37</v>
       </c>
       <c r="F11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -10436,7 +10436,7 @@
         <v>37</v>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -10472,7 +10472,7 @@
         <v>37</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -10679,7 +10679,7 @@
         <v>37</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -10711,7 +10711,7 @@
         <v>37</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -10747,7 +10747,7 @@
         <v>37</v>
       </c>
       <c r="F25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -10875,7 +10875,7 @@
         <v>37</v>
       </c>
       <c r="F30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
@@ -11078,7 +11078,7 @@
         <v>37</v>
       </c>
       <c r="F38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
@@ -11135,7 +11135,7 @@
         <v>37</v>
       </c>
       <c r="F40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
@@ -11197,7 +11197,7 @@
         <v>37</v>
       </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
tests: Finish test uploading to CDF
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59381834-3652-49EC-87E8-A7FF298D3CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2774A3-6FE8-45C3-9AB9-ED71C093415E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="111">
   <si>
     <t>role</t>
   </si>
@@ -129,9 +129,6 @@
     <t>timeseries</t>
   </si>
   <si>
-    <t>CircuitBreaker</t>
-  </si>
-  <si>
     <t>WindFarm</t>
   </si>
   <si>
@@ -210,49 +207,22 @@
     <t>power:OffshoreSubstation</t>
   </si>
   <si>
-    <t>TransmissionSubstation</t>
-  </si>
-  <si>
-    <t>DistributionSubstation</t>
-  </si>
-  <si>
     <t>PowerLine</t>
   </si>
   <si>
     <t>power:PowerLine</t>
   </si>
   <si>
-    <t>ArrayCable</t>
-  </si>
-  <si>
     <t>power:ArrayCable</t>
   </si>
   <si>
-    <t>ExportCable</t>
-  </si>
-  <si>
     <t>power:ExportCable</t>
-  </si>
-  <si>
-    <t>Transmission</t>
-  </si>
-  <si>
-    <t>EnergyConsumer</t>
-  </si>
-  <si>
-    <t>power:EnergyConsumer</t>
   </si>
   <si>
     <t>Factory</t>
   </si>
   <si>
     <t>power:Factory</t>
-  </si>
-  <si>
-    <t>GeoLocation</t>
-  </si>
-  <si>
-    <t>power:GeoLocation</t>
   </si>
   <si>
     <t>Point</t>
@@ -276,25 +246,13 @@
     <t>power:CircuitBreaker</t>
   </si>
   <si>
-    <t>CurrentTransformer</t>
-  </si>
-  <si>
     <t>power:CurrentTransformer</t>
-  </si>
-  <si>
-    <t>DisconnectSwitch</t>
   </si>
   <si>
     <t>power:DisconnectSwitch</t>
   </si>
   <si>
-    <t>VoltageLevel</t>
-  </si>
-  <si>
     <t>power:VoltageLevel</t>
-  </si>
-  <si>
-    <t>VoltageTransformer</t>
   </si>
   <si>
     <t>power:VoltageTransformer</t>
@@ -403,42 +361,6 @@
   </si>
   <si>
     <t>windTurbines</t>
-  </si>
-  <si>
-    <t>power:TransmissionSubstation(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:DistributionSubstation(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:ArrayCable(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:ExportCable(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:Transmission(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:EnergyConsumer(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:GeoLocation(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:CircuitBreaker(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:CurrentTransformer(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:DisconnectSwitch(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:VoltageLevel(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:VoltageTransformer(version=0.1.0)</t>
   </si>
 </sst>
 </file>
@@ -891,10 +813,10 @@
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -931,7 +853,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -957,7 +879,7 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="5"/>
@@ -984,10 +906,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1016,7 +938,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1042,10 +964,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1071,7 +993,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="15">
         <v>45351.489040733439</v>
@@ -8728,10 +8650,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X1000"/>
+  <dimension ref="A1:X993"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8747,7 +8669,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="20"/>
@@ -8784,7 +8706,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -8795,7 +8717,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -8804,223 +8726,111 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>100</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9982,13 +9792,6 @@
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -10005,8 +9808,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10125,19 +9928,19 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" t="s">
         <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
@@ -10151,7 +9954,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -10163,19 +9966,19 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="N4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
@@ -10200,13 +10003,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M5" t="s">
         <v>30</v>
@@ -10221,13 +10024,13 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -10236,19 +10039,19 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
@@ -10278,13 +10081,13 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K8" t="s">
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M8" t="s">
         <v>26</v>
@@ -10311,13 +10114,13 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
         <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M9" t="s">
         <v>27</v>
@@ -10340,13 +10143,13 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K10" t="s">
         <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M10" t="s">
         <v>31</v>
@@ -10361,13 +10164,13 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -10376,16 +10179,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="L11" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M11" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
@@ -10397,10 +10200,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -10409,31 +10212,31 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="L12" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -10442,16 +10245,16 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
@@ -10460,16 +10263,16 @@
     </row>
     <row r="15" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -10478,16 +10281,16 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="L15" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
@@ -10496,10 +10299,10 @@
     </row>
     <row r="16" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -10511,16 +10314,16 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="L16" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -10535,7 +10338,7 @@
     </row>
     <row r="18" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
@@ -10550,13 +10353,13 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K18" t="s">
         <v>23</v>
       </c>
       <c r="L18" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M18" t="s">
         <v>23</v>
@@ -10568,7 +10371,7 @@
     </row>
     <row r="19" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -10583,13 +10386,13 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K19" t="s">
         <v>25</v>
       </c>
       <c r="L19" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M19" t="s">
         <v>25</v>
@@ -10597,22 +10400,22 @@
     </row>
     <row r="20" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L20" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M20" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
@@ -10621,22 +10424,22 @@
     </row>
     <row r="21" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L21" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
@@ -10645,38 +10448,38 @@
     </row>
     <row r="22" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L22" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M22" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" t="s">
-        <v>37</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -10685,30 +10488,30 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K23" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="L23" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M23" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
         <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -10717,16 +10520,16 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K24" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="L24" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M24" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
@@ -10735,16 +10538,16 @@
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -10753,16 +10556,16 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K25" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="L25" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M25" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
@@ -10771,10 +10574,10 @@
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -10786,24 +10589,24 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="L26" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -10815,16 +10618,16 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K27" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="L27" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M27" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
@@ -10839,22 +10642,22 @@
     </row>
     <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L29" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="M29" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
@@ -10863,16 +10666,16 @@
     </row>
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -10881,16 +10684,16 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K30" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="L30" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="M30" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
@@ -10905,7 +10708,7 @@
     </row>
     <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -10920,13 +10723,13 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K32" t="s">
         <v>23</v>
       </c>
       <c r="L32" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M32" t="s">
         <v>23</v>
@@ -10938,16 +10741,16 @@
     </row>
     <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
@@ -10956,16 +10759,16 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="L33" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="R33" s="11"/>
       <c r="S33" s="11"/>
@@ -10974,7 +10777,7 @@
     </row>
     <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
         <v>27</v>
@@ -10989,13 +10792,13 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K34" t="s">
         <v>27</v>
       </c>
       <c r="L34" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M34" t="s">
         <v>27</v>
@@ -11003,7 +10806,7 @@
     </row>
     <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
@@ -11018,13 +10821,13 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K35" t="s">
         <v>30</v>
       </c>
       <c r="L35" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M35" t="s">
         <v>30</v>
@@ -11042,22 +10845,22 @@
     </row>
     <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" t="s">
         <v>34</v>
       </c>
-      <c r="B37" t="s">
-        <v>124</v>
-      </c>
-      <c r="D37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" t="s">
-        <v>35</v>
-      </c>
       <c r="L37" t="s">
+        <v>96</v>
+      </c>
+      <c r="M37" t="s">
         <v>110</v>
-      </c>
-      <c r="M37" t="s">
-        <v>124</v>
       </c>
       <c r="R37" s="10"/>
       <c r="S37" s="11"/>
@@ -11066,16 +10869,16 @@
     </row>
     <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -11084,16 +10887,16 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="L38" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="R38" s="10"/>
       <c r="S38" s="11"/>
@@ -11102,37 +10905,37 @@
     </row>
     <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" t="s">
         <v>34</v>
       </c>
-      <c r="B39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" t="s">
-        <v>35</v>
-      </c>
       <c r="L39" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M39" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="R39" s="10"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
@@ -11141,22 +10944,22 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K40" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="L40" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M40" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
@@ -11171,13 +10974,13 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K42" t="s">
         <v>23</v>
       </c>
       <c r="L42" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="M42" t="s">
         <v>23</v>
@@ -11185,16 +10988,16 @@
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -11203,13 +11006,13 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K43" t="s">
         <v>25</v>
       </c>
       <c r="L43" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="M43" t="s">
         <v>25</v>
@@ -11217,10 +11020,10 @@
     </row>
     <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -11232,25 +11035,25 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K44" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="L44" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
         <v>28</v>
@@ -11262,24 +11065,24 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K46" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="L46" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="M46" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
         <v>28</v>
@@ -11291,69 +11094,70 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K47" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="L47" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="M47" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L49" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="M49" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+      <c r="L50" t="s">
+        <v>107</v>
+      </c>
+      <c r="M50" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="D51" t="s">
-        <v>76</v>
-      </c>
-      <c r="E51" t="s">
-        <v>35</v>
-      </c>
-      <c r="L51" t="s">
-        <v>121</v>
-      </c>
-      <c r="M51" t="s">
-        <v>119</v>
-      </c>
+      <c r="C51" s="12"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="12"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
@@ -23829,7 +23633,7 @@
   <dimension ref="A1:X1004"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23845,7 +23649,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -23893,83 +23697,84 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
-        <v>59</v>
-      </c>
       <c r="D8" t="s">
-        <v>57</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactor; updated Alice with all views and containers
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2774A3-6FE8-45C3-9AB9-ED71C093415E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44ED5FB-C2AF-4F51-BBA6-8E0006FB8CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="130">
   <si>
     <t>role</t>
   </si>
@@ -361,6 +361,63 @@
   </si>
   <si>
     <t>windTurbines</t>
+  </si>
+  <si>
+    <t>CurrentTransformer</t>
+  </si>
+  <si>
+    <t>maxCapacity</t>
+  </si>
+  <si>
+    <t>VoltageTransformer</t>
+  </si>
+  <si>
+    <t>outputVoltageLevel</t>
+  </si>
+  <si>
+    <t>inputVoltageLevel</t>
+  </si>
+  <si>
+    <t>VoltageLevel</t>
+  </si>
+  <si>
+    <t>maxLevel</t>
+  </si>
+  <si>
+    <t>ExportCable</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>CircuitBreaker</t>
+  </si>
+  <si>
+    <t>ArrayCable</t>
+  </si>
+  <si>
+    <t>DisconnectSwitch</t>
+  </si>
+  <si>
+    <t>power:CurrentTransformer(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:VoltageTransformer(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:VoltageLevel(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:ExportCable(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:CircuitBreaker(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:ArrayCable(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:DisconnectSwitch(version=0.1.0)</t>
   </si>
 </sst>
 </file>
@@ -8652,8 +8709,8 @@
   </sheetPr>
   <dimension ref="A1:X993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8813,24 +8870,74 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9808,8 +9915,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9820,7 +9927,7 @@
     <col min="4" max="4" width="30.109375" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.44140625" customWidth="1"/>
     <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -11158,98 +11265,256 @@
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M52" s="9"/>
+      <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>72</v>
+      </c>
+      <c r="K52" t="s">
+        <v>112</v>
+      </c>
+      <c r="L52" t="s">
+        <v>123</v>
+      </c>
+      <c r="M52" t="s">
+        <v>112</v>
+      </c>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="12"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>75</v>
+      </c>
+      <c r="K53" t="s">
+        <v>114</v>
+      </c>
+      <c r="L53" t="s">
+        <v>124</v>
+      </c>
+      <c r="M53" t="s">
+        <v>114</v>
+      </c>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="12"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>75</v>
+      </c>
+      <c r="K54" t="s">
+        <v>115</v>
+      </c>
+      <c r="L54" t="s">
+        <v>124</v>
+      </c>
+      <c r="M54" t="s">
+        <v>115</v>
+      </c>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="12"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>74</v>
+      </c>
+      <c r="K55" t="s">
+        <v>117</v>
+      </c>
+      <c r="L55" t="s">
+        <v>125</v>
+      </c>
+      <c r="M55" t="s">
+        <v>117</v>
+      </c>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="12"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="9"/>
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>62</v>
+      </c>
+      <c r="K56" t="s">
+        <v>119</v>
+      </c>
+      <c r="L56" t="s">
+        <v>126</v>
+      </c>
+      <c r="M56" t="s">
+        <v>119</v>
+      </c>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
     </row>
     <row r="57" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="12"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
+      <c r="A57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>71</v>
+      </c>
+      <c r="K57" t="s">
+        <v>112</v>
+      </c>
+      <c r="L57" t="s">
+        <v>127</v>
+      </c>
+      <c r="M57" t="s">
+        <v>112</v>
+      </c>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
     </row>
     <row r="58" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="12"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>61</v>
+      </c>
+      <c r="K58" t="s">
+        <v>119</v>
+      </c>
+      <c r="L58" t="s">
+        <v>128</v>
+      </c>
+      <c r="M58" t="s">
+        <v>119</v>
+      </c>
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
     </row>
     <row r="59" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="12"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>73</v>
+      </c>
+      <c r="K59" t="s">
+        <v>112</v>
+      </c>
+      <c r="L59" t="s">
+        <v>129</v>
+      </c>
+      <c r="M59" t="s">
+        <v>112</v>
+      </c>
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
     </row>
@@ -23632,8 +23897,8 @@
   </sheetPr>
   <dimension ref="A1:X1004"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23777,17 +24042,69 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[NEAT-41] Export to CDF and Integration Test (#283)
* refactor: shell for export_to_cdf

* refactor: export to CDF

* refactor; added options

* refactor: more options for DMSExporter

* fix: Alice direct nullable

* tests: Finish test uploading to CDF

* feat: Added check that all classes has defined properties

* refactor; updated Alice with all views and containers

* refactor; moved over CDF loaders

* refactor; NoParent

* refactor; renaming _data_classes to _models
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E11DB8C-5CB4-45E7-B56C-6B8BE8DD01D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44ED5FB-C2AF-4F51-BBA6-8E0006FB8CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="130">
   <si>
     <t>role</t>
   </si>
@@ -129,9 +129,6 @@
     <t>timeseries</t>
   </si>
   <si>
-    <t>CircuitBreaker</t>
-  </si>
-  <si>
     <t>WindFarm</t>
   </si>
   <si>
@@ -210,49 +207,22 @@
     <t>power:OffshoreSubstation</t>
   </si>
   <si>
-    <t>TransmissionSubstation</t>
-  </si>
-  <si>
-    <t>DistributionSubstation</t>
-  </si>
-  <si>
     <t>PowerLine</t>
   </si>
   <si>
     <t>power:PowerLine</t>
   </si>
   <si>
-    <t>ArrayCable</t>
-  </si>
-  <si>
     <t>power:ArrayCable</t>
   </si>
   <si>
-    <t>ExportCable</t>
-  </si>
-  <si>
     <t>power:ExportCable</t>
-  </si>
-  <si>
-    <t>Transmission</t>
-  </si>
-  <si>
-    <t>EnergyConsumer</t>
-  </si>
-  <si>
-    <t>power:EnergyConsumer</t>
   </si>
   <si>
     <t>Factory</t>
   </si>
   <si>
     <t>power:Factory</t>
-  </si>
-  <si>
-    <t>GeoLocation</t>
-  </si>
-  <si>
-    <t>power:GeoLocation</t>
   </si>
   <si>
     <t>Point</t>
@@ -276,25 +246,13 @@
     <t>power:CircuitBreaker</t>
   </si>
   <si>
-    <t>CurrentTransformer</t>
-  </si>
-  <si>
     <t>power:CurrentTransformer</t>
-  </si>
-  <si>
-    <t>DisconnectSwitch</t>
   </si>
   <si>
     <t>power:DisconnectSwitch</t>
   </si>
   <si>
-    <t>VoltageLevel</t>
-  </si>
-  <si>
     <t>power:VoltageLevel</t>
-  </si>
-  <si>
-    <t>VoltageTransformer</t>
   </si>
   <si>
     <t>power:VoltageTransformer</t>
@@ -405,40 +363,61 @@
     <t>windTurbines</t>
   </si>
   <si>
-    <t>power:TransmissionSubstation(version=0.1.0)</t>
+    <t>CurrentTransformer</t>
   </si>
   <si>
-    <t>power:DistributionSubstation(version=0.1.0)</t>
+    <t>maxCapacity</t>
+  </si>
+  <si>
+    <t>VoltageTransformer</t>
+  </si>
+  <si>
+    <t>outputVoltageLevel</t>
+  </si>
+  <si>
+    <t>inputVoltageLevel</t>
+  </si>
+  <si>
+    <t>VoltageLevel</t>
+  </si>
+  <si>
+    <t>maxLevel</t>
+  </si>
+  <si>
+    <t>ExportCable</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>CircuitBreaker</t>
+  </si>
+  <si>
+    <t>ArrayCable</t>
+  </si>
+  <si>
+    <t>DisconnectSwitch</t>
+  </si>
+  <si>
+    <t>power:CurrentTransformer(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:VoltageTransformer(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:VoltageLevel(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:ExportCable(version=0.1.0)</t>
+  </si>
+  <si>
+    <t>power:CircuitBreaker(version=0.1.0)</t>
   </si>
   <si>
     <t>power:ArrayCable(version=0.1.0)</t>
   </si>
   <si>
-    <t>power:ExportCable(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:Transmission(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:EnergyConsumer(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:GeoLocation(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:CircuitBreaker(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:CurrentTransformer(version=0.1.0)</t>
-  </si>
-  <si>
     <t>power:DisconnectSwitch(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:VoltageLevel(version=0.1.0)</t>
-  </si>
-  <si>
-    <t>power:VoltageTransformer(version=0.1.0)</t>
   </si>
 </sst>
 </file>
@@ -891,10 +870,10 @@
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -931,7 +910,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -957,7 +936,7 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="5"/>
@@ -984,10 +963,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1016,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1042,10 +1021,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1071,7 +1050,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="15">
         <v>45351.489040733439</v>
@@ -8728,10 +8707,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X1000"/>
+  <dimension ref="A1:X993"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8747,7 +8726,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="20"/>
@@ -8784,7 +8763,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -8795,7 +8774,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -8804,223 +8783,161 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>100</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
         <v>129</v>
       </c>
-      <c r="D14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9982,13 +9899,6 @@
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -10005,8 +9915,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10017,7 +9927,7 @@
     <col min="4" max="4" width="30.109375" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.44140625" customWidth="1"/>
     <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -10125,19 +10035,19 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" t="s">
         <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
@@ -10151,7 +10061,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -10163,19 +10073,19 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="N4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
@@ -10200,13 +10110,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M5" t="s">
         <v>30</v>
@@ -10221,34 +10131,34 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="M6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
@@ -10278,13 +10188,13 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K8" t="s">
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M8" t="s">
         <v>26</v>
@@ -10311,13 +10221,13 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
         <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M9" t="s">
         <v>27</v>
@@ -10340,13 +10250,13 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K10" t="s">
         <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M10" t="s">
         <v>31</v>
@@ -10361,31 +10271,31 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="L11" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M11" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
@@ -10397,10 +10307,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -10409,49 +10319,49 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="L12" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="M12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
@@ -10460,34 +10370,34 @@
     </row>
     <row r="15" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="L15" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
@@ -10496,10 +10406,10 @@
     </row>
     <row r="16" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -10511,16 +10421,16 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="L16" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -10535,7 +10445,7 @@
     </row>
     <row r="18" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
@@ -10550,13 +10460,13 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K18" t="s">
         <v>23</v>
       </c>
       <c r="L18" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M18" t="s">
         <v>23</v>
@@ -10568,7 +10478,7 @@
     </row>
     <row r="19" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -10583,13 +10493,13 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K19" t="s">
         <v>25</v>
       </c>
       <c r="L19" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M19" t="s">
         <v>25</v>
@@ -10597,22 +10507,22 @@
     </row>
     <row r="20" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L20" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M20" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
@@ -10621,22 +10531,22 @@
     </row>
     <row r="21" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L21" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
@@ -10645,88 +10555,88 @@
     </row>
     <row r="22" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L22" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M22" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" t="s">
-        <v>37</v>
-      </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K23" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="L23" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M23" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
-      </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K24" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="L24" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M24" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
@@ -10735,34 +10645,34 @@
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
-      </c>
       <c r="F25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K25" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="L25" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M25" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
@@ -10771,10 +10681,10 @@
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -10786,24 +10696,24 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="L26" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -10815,16 +10725,16 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K27" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="L27" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M27" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
@@ -10839,22 +10749,22 @@
     </row>
     <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L29" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="M29" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
@@ -10863,34 +10773,34 @@
     </row>
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K30" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="L30" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="M30" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
@@ -10905,7 +10815,7 @@
     </row>
     <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -10920,13 +10830,13 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K32" t="s">
         <v>23</v>
       </c>
       <c r="L32" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M32" t="s">
         <v>23</v>
@@ -10938,16 +10848,16 @@
     </row>
     <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
@@ -10956,16 +10866,16 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="L33" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="R33" s="11"/>
       <c r="S33" s="11"/>
@@ -10974,7 +10884,7 @@
     </row>
     <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
         <v>27</v>
@@ -10989,13 +10899,13 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K34" t="s">
         <v>27</v>
       </c>
       <c r="L34" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M34" t="s">
         <v>27</v>
@@ -11003,7 +10913,7 @@
     </row>
     <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
@@ -11018,13 +10928,13 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K35" t="s">
         <v>30</v>
       </c>
       <c r="L35" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="M35" t="s">
         <v>30</v>
@@ -11042,22 +10952,22 @@
     </row>
     <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" t="s">
         <v>34</v>
       </c>
-      <c r="B37" t="s">
-        <v>124</v>
-      </c>
-      <c r="D37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" t="s">
-        <v>35</v>
-      </c>
       <c r="L37" t="s">
+        <v>96</v>
+      </c>
+      <c r="M37" t="s">
         <v>110</v>
-      </c>
-      <c r="M37" t="s">
-        <v>124</v>
       </c>
       <c r="R37" s="10"/>
       <c r="S37" s="11"/>
@@ -11066,34 +10976,34 @@
     </row>
     <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="L38" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="R38" s="10"/>
       <c r="S38" s="11"/>
@@ -11102,61 +11012,61 @@
     </row>
     <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" t="s">
         <v>34</v>
       </c>
-      <c r="B39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" t="s">
-        <v>35</v>
-      </c>
       <c r="L39" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M39" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="R39" s="10"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K40" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="L40" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M40" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
@@ -11171,13 +11081,13 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K42" t="s">
         <v>23</v>
       </c>
       <c r="L42" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="M42" t="s">
         <v>23</v>
@@ -11185,31 +11095,31 @@
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K43" t="s">
         <v>25</v>
       </c>
       <c r="L43" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="M43" t="s">
         <v>25</v>
@@ -11217,10 +11127,10 @@
     </row>
     <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -11232,25 +11142,25 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K44" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="L44" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
         <v>28</v>
@@ -11262,24 +11172,24 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K46" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="L46" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="M46" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
         <v>28</v>
@@ -11291,161 +11201,320 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K47" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="L47" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="M47" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L49" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="M49" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+      <c r="L50" t="s">
+        <v>107</v>
+      </c>
+      <c r="M50" t="s">
+        <v>105</v>
+      </c>
+    </row>
     <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="D51" t="s">
-        <v>76</v>
-      </c>
-      <c r="E51" t="s">
-        <v>35</v>
-      </c>
-      <c r="L51" t="s">
-        <v>121</v>
-      </c>
-      <c r="M51" t="s">
-        <v>119</v>
-      </c>
+      <c r="C51" s="12"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="12"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
+      <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>72</v>
+      </c>
+      <c r="K52" t="s">
+        <v>112</v>
+      </c>
+      <c r="L52" t="s">
+        <v>123</v>
+      </c>
+      <c r="M52" t="s">
+        <v>112</v>
+      </c>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="12"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>75</v>
+      </c>
+      <c r="K53" t="s">
+        <v>114</v>
+      </c>
+      <c r="L53" t="s">
+        <v>124</v>
+      </c>
+      <c r="M53" t="s">
+        <v>114</v>
+      </c>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="12"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>75</v>
+      </c>
+      <c r="K54" t="s">
+        <v>115</v>
+      </c>
+      <c r="L54" t="s">
+        <v>124</v>
+      </c>
+      <c r="M54" t="s">
+        <v>115</v>
+      </c>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="12"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>74</v>
+      </c>
+      <c r="K55" t="s">
+        <v>117</v>
+      </c>
+      <c r="L55" t="s">
+        <v>125</v>
+      </c>
+      <c r="M55" t="s">
+        <v>117</v>
+      </c>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="12"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="9"/>
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>62</v>
+      </c>
+      <c r="K56" t="s">
+        <v>119</v>
+      </c>
+      <c r="L56" t="s">
+        <v>126</v>
+      </c>
+      <c r="M56" t="s">
+        <v>119</v>
+      </c>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
     </row>
     <row r="57" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="12"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
+      <c r="A57" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>71</v>
+      </c>
+      <c r="K57" t="s">
+        <v>112</v>
+      </c>
+      <c r="L57" t="s">
+        <v>127</v>
+      </c>
+      <c r="M57" t="s">
+        <v>112</v>
+      </c>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
     </row>
     <row r="58" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="12"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>61</v>
+      </c>
+      <c r="K58" t="s">
+        <v>119</v>
+      </c>
+      <c r="L58" t="s">
+        <v>128</v>
+      </c>
+      <c r="M58" t="s">
+        <v>119</v>
+      </c>
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
     </row>
     <row r="59" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="12"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>73</v>
+      </c>
+      <c r="K59" t="s">
+        <v>112</v>
+      </c>
+      <c r="L59" t="s">
+        <v>129</v>
+      </c>
+      <c r="M59" t="s">
+        <v>112</v>
+      </c>
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
     </row>
@@ -23828,8 +23897,8 @@
   </sheetPr>
   <dimension ref="A1:X1004"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23845,7 +23914,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -23893,96 +23962,149 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
-        <v>59</v>
-      </c>
       <c r="D8" t="s">
-        <v>57</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
         <v>75</v>
       </c>
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[NEAT-67] Renaming Source to Reference (#303)
* refactor: Rename source to reference

* refactor; update spreadsheets
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/cdf-dms-architect-alice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB7892F-7BB4-49EE-97BB-EA2BD8EC1426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264EA5D0-BCE9-4FF8-945D-4CF7980E82A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Default</t>
-  </si>
-  <si>
-    <t>Source</t>
   </si>
   <si>
     <t>Container</t>
@@ -413,6 +410,9 @@
   <si>
     <t>power:DisconnectSwitch(version=0.1.0)</t>
   </si>
+  <si>
+    <t>Reference</t>
+  </si>
 </sst>
 </file>
 
@@ -617,6 +617,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -631,7 +632,6 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,7 +852,7 @@
   </sheetPr>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -880,10 +880,10 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -917,10 +917,10 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -946,7 +946,7 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="5"/>
@@ -973,10 +973,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1005,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1031,10 +1031,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="15">
         <v>45351.489040733439</v>
@@ -8735,12 +8735,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -8767,13 +8767,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -8781,159 +8781,159 @@
     </row>
     <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9925,8 +9925,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9936,7 +9936,8 @@
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="9" width="13.140625" customWidth="1"/>
+    <col min="6" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="37.42578125" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
@@ -9955,23 +9956,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -9999,25 +10000,25 @@
         <v>14</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -10030,13 +10031,13 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -10045,19 +10046,19 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
@@ -10068,13 +10069,13 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -10083,19 +10084,19 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" t="s">
         <v>74</v>
       </c>
-      <c r="M4" t="s">
-        <v>75</v>
-      </c>
       <c r="N4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
@@ -10105,13 +10106,13 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -10120,16 +10121,16 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
@@ -10138,16 +10139,16 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -10156,19 +10157,19 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
@@ -10183,13 +10184,13 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -10198,16 +10199,16 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
@@ -10216,13 +10217,13 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -10231,27 +10232,27 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -10260,16 +10261,16 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -10278,16 +10279,16 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -10296,16 +10297,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L11" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" t="s">
         <v>78</v>
-      </c>
-      <c r="M11" t="s">
-        <v>79</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
@@ -10314,13 +10315,13 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" t="s">
         <v>80</v>
-      </c>
-      <c r="D12" t="s">
-        <v>81</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -10329,31 +10330,31 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -10362,16 +10363,16 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
@@ -10380,16 +10381,16 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -10398,16 +10399,16 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
@@ -10416,13 +10417,13 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -10431,16 +10432,16 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L16" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" t="s">
         <v>82</v>
-      </c>
-      <c r="M16" t="s">
-        <v>83</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -10455,13 +10456,13 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
         <v>23</v>
-      </c>
-      <c r="D18" t="s">
-        <v>24</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -10470,16 +10471,16 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
@@ -10488,13 +10489,13 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -10503,36 +10504,36 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L20" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20" t="s">
         <v>84</v>
-      </c>
-      <c r="M20" t="s">
-        <v>85</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
@@ -10541,22 +10542,22 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
@@ -10565,38 +10566,38 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -10605,30 +10606,30 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" t="s">
-        <v>36</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -10637,16 +10638,16 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
@@ -10655,16 +10656,16 @@
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" t="s">
         <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" t="s">
-        <v>36</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -10673,16 +10674,16 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
@@ -10691,13 +10692,13 @@
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -10706,27 +10707,27 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -10735,16 +10736,16 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
@@ -10759,22 +10760,22 @@
     </row>
     <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
@@ -10783,16 +10784,16 @@
     </row>
     <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -10801,16 +10802,16 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
@@ -10825,13 +10826,13 @@
     </row>
     <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
         <v>23</v>
-      </c>
-      <c r="D32" t="s">
-        <v>24</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -10840,16 +10841,16 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R32" s="11"/>
       <c r="S32" s="11"/>
@@ -10858,16 +10859,16 @@
     </row>
     <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
@@ -10876,16 +10877,16 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R33" s="11"/>
       <c r="S33" s="11"/>
@@ -10894,13 +10895,13 @@
     </row>
     <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
         <v>27</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -10909,27 +10910,27 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -10938,16 +10939,16 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R35" s="10"/>
       <c r="S35" s="11"/>
@@ -10962,22 +10963,22 @@
     </row>
     <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
         <v>33</v>
       </c>
-      <c r="B37" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
       <c r="L37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R37" s="10"/>
       <c r="S37" s="11"/>
@@ -10986,16 +10987,16 @@
     </row>
     <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -11004,16 +11005,16 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L38" t="s">
+        <v>93</v>
+      </c>
+      <c r="M38" t="s">
         <v>94</v>
-      </c>
-      <c r="M38" t="s">
-        <v>95</v>
       </c>
       <c r="R38" s="10"/>
       <c r="S38" s="11"/>
@@ -11022,37 +11023,37 @@
     </row>
     <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" t="s">
         <v>33</v>
       </c>
-      <c r="B39" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
       <c r="L39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R39" s="10"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
@@ -11061,28 +11062,28 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
         <v>23</v>
-      </c>
-      <c r="D42" t="s">
-        <v>24</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -11091,30 +11092,30 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>101</v>
+        <v>24</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="E43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -11123,27 +11124,27 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -11152,28 +11153,28 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L44" t="s">
+        <v>97</v>
+      </c>
+      <c r="M44" t="s">
         <v>98</v>
-      </c>
-      <c r="M44" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -11182,27 +11183,27 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K46" t="s">
+        <v>99</v>
+      </c>
+      <c r="L46" t="s">
         <v>100</v>
       </c>
-      <c r="L46" t="s">
-        <v>101</v>
-      </c>
       <c r="M46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -11211,57 +11212,57 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L47" t="s">
+        <v>100</v>
+      </c>
+      <c r="M47" t="s">
         <v>101</v>
-      </c>
-      <c r="M47" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+      <c r="L49" t="s">
         <v>103</v>
       </c>
-      <c r="D49" t="s">
-        <v>101</v>
-      </c>
-      <c r="E49" t="s">
-        <v>34</v>
-      </c>
-      <c r="L49" t="s">
-        <v>104</v>
-      </c>
       <c r="M49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11276,13 +11277,13 @@
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
         <v>109</v>
       </c>
-      <c r="B52" t="s">
-        <v>110</v>
-      </c>
       <c r="D52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
@@ -11291,32 +11292,32 @@
         <v>0</v>
       </c>
       <c r="J52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
         <v>111</v>
       </c>
-      <c r="B53" t="s">
-        <v>112</v>
-      </c>
       <c r="D53" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
@@ -11325,32 +11326,32 @@
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F54" t="b">
         <v>1</v>
@@ -11359,29 +11360,29 @@
         <v>0</v>
       </c>
       <c r="J54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" t="s">
         <v>114</v>
       </c>
-      <c r="B55" t="s">
-        <v>115</v>
-      </c>
       <c r="D55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
@@ -11390,29 +11391,29 @@
         <v>0</v>
       </c>
       <c r="J55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" t="s">
         <v>116</v>
       </c>
-      <c r="B56" t="s">
-        <v>117</v>
-      </c>
       <c r="D56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
@@ -11421,29 +11422,29 @@
         <v>0</v>
       </c>
       <c r="J56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
     </row>
     <row r="57" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -11452,29 +11453,29 @@
         <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
     </row>
     <row r="58" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F58" t="b">
         <v>1</v>
@@ -11483,29 +11484,29 @@
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
     </row>
     <row r="59" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
@@ -11514,16 +11515,16 @@
         <v>0</v>
       </c>
       <c r="J59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
@@ -23923,12 +23924,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="24"/>
+      <c r="A1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -23955,13 +23956,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -23969,143 +23970,143 @@
     </row>
     <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
       </c>
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
         <v>57</v>
       </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
         <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>